<commit_message>
Change SPARQL path parsing
</commit_message>
<xml_diff>
--- a/xls2rdf-lib/src/test/resources/suite/_50_sparqlToShaclPath/input.xlsx
+++ b/xls2rdf-lib/src/test/resources/suite/_50_sparqlToShaclPath/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">URI of ConceptScheme</t>
   </si>
@@ -34,7 +34,7 @@
     <t>skos:prefLabel@fr</t>
   </si>
   <si>
-    <t>sh:path(sparqlPathToShacl="true")</t>
+    <t>sh:path</t>
   </si>
   <si>
     <t>http://labs.sparna.fr/skos-play/convert/test/concept_1</t>
@@ -53,16 +53,40 @@
   </si>
   <si>
     <t>hide</t>
+  </si>
+  <si>
+    <t>http://labs.sparna.fr/skos-play/convert/test/concept_2</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>skos:broader</t>
+  </si>
+  <si>
+    <t>http://labs.sparna.fr/skos-play/convert/test/concept_3</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>http://labs.sparna.fr/skos-play/convert/test/concept_4</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[sh:inversePath skos:broader]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode=""/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
@@ -88,6 +112,12 @@
       <color indexed="4"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10.000000"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -108,13 +138,13 @@
   </borders>
   <cellStyleXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -126,6 +156,7 @@
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -646,10 +677,10 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -662,6 +693,39 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -673,6 +737,9 @@
     <hyperlink r:id="rId2" ref="B4"/>
     <hyperlink r:id="rId3" ref="A5"/>
     <hyperlink r:id="rId4" ref="A6"/>
+    <hyperlink r:id="rId5" ref="A7"/>
+    <hyperlink r:id="rId6" ref="A8"/>
+    <hyperlink r:id="rId7" ref="A9"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.052778" bottom="1.052778" header="0.78750000000000009" footer="0.78750000000000009"/>

</xml_diff>